<commit_message>
feat(data): :sparkles: update historical data and enhance StudyAreaPage
- Updated `historical_data.json` to extend the range of years and include additional data points for sediment load and forest coverage.
- Modified `StudyAreaPage` to set the default year to 2020, aligning with the updated historical data.
- Updated binary files: `sediment.xlsx` and `forest_coverage_historical.parquet` to reflect the latest data changes.
</commit_message>
<xml_diff>
--- a/sediment.xlsx
+++ b/sediment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songshgeo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694AD0F5-8D4D-B049-BD73-87B907B67056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA8367-4BB7-9F4A-86B4-4C800EA6677E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{831DCF93-1576-D649-BB22-682F215EEAD6}"/>
   </bookViews>
@@ -1317,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAC5C04-0CD4-E84B-8853-955BD281F4B2}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2296,6 +2296,246 @@
         <v>7.5557365000000001E-2</v>
       </c>
     </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B122" s="1">
+        <v>9.2437438999999996E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B123" s="1">
+        <v>9.2759037000000003E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B124" s="1">
+        <v>9.3386048999999999E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B125" s="1">
+        <v>9.3757749000000001E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B126" s="1">
+        <v>9.4563718000000005E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B127" s="1">
+        <v>9.5301708999999998E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B128" s="1">
+        <v>9.5933589999999999E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B129" s="1">
+        <v>9.6374731000000005E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B130" s="1">
+        <v>9.6559106000000006E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B131" s="1">
+        <v>9.6564838E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B132" s="1">
+        <v>9.6685108000000006E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B133" s="1">
+        <v>9.6855833000000002E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B134" s="1">
+        <v>9.7477267000000006E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B135" s="1">
+        <v>9.8103177999999999E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B136" s="1">
+        <v>9.9019310999999999E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0.100250851</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0.101453266</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B139" s="1">
+        <v>0.10213665199999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0.102838016</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0.10339466999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B142" s="1">
+        <v>0.104658512</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B143" s="1">
+        <v>0.105491901</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0.106636957</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0.107014838</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0.107658669</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0.108301522</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0.10982653100000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0.11090301700000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0.11170989000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.112605549</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>